<commit_message>
Ajustar vista colores y logo corporativo
</commit_message>
<xml_diff>
--- a/resultados_rifa_set_1.xlsx
+++ b/resultados_rifa_set_1.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -463,38 +463,23 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>BAUTISTA BAUTISTA MARGORI DEL CARMEN</t>
+          <t>MARQUEZ GONZALEZ CARLOS DANIEL</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>BERA SALUD</t>
+          <t>BERA OUTLET</t>
         </is>
       </c>
       <c r="C2" t="b">
         <v>1</v>
       </c>
-      <c r="D2" t="inlineStr"/>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Licuadora</t>
+        </is>
+      </c>
       <c r="E2" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>MORALES TORRES LUIS ENRIQUE</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>BERA I</t>
-        </is>
-      </c>
-      <c r="C3" t="b">
-        <v>1</v>
-      </c>
-      <c r="D3" t="inlineStr"/>
-      <c r="E3" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>